<commit_message>
Changes in the submit ico details steps
</commit_message>
<xml_diff>
--- a/TestData/BullTokenTestData.xlsx
+++ b/TestData/BullTokenTestData.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18588" windowHeight="4860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18588" windowHeight="7632" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
     <sheet name="ICOBasicDetail" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G4"/>
+  <oleSize ref="A1:G1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>TestCase</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Valid LoginCredentials</t>
   </si>
   <si>
-    <t>ajmera@test.com</t>
-  </si>
-  <si>
     <t>Password123</t>
   </si>
   <si>
@@ -123,6 +120,27 @@
   </si>
   <si>
     <t>https://github.com/abhina.com</t>
+  </si>
+  <si>
+    <t>ContactEmail</t>
+  </si>
+  <si>
+    <t>ContactAddress</t>
+  </si>
+  <si>
+    <t>ContactNumber</t>
+  </si>
+  <si>
+    <t>info@bullcom.com</t>
+  </si>
+  <si>
+    <t>Test address</t>
+  </si>
+  <si>
+    <t>ygupta5056@gmail.com</t>
+  </si>
+  <si>
+    <t>akshat01@test.com</t>
   </si>
 </sst>
 </file>
@@ -482,13 +500,13 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -508,10 +526,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -519,7 +537,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>3</v>
@@ -533,7 +551,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -543,21 +561,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{5387E9B4-E56A-420C-9301-23D419074B56}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{BF3BE161-5167-48B4-8892-0770BFB83026}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{1B395A58-D2BF-4C5F-BAAA-794DC28A96B4}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{BF3BE161-5167-48B4-8892-0770BFB83026}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{1B395A58-D2BF-4C5F-BAAA-794DC28A96B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F16B26-84A7-47A5-8419-0CD2AD22C342}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,82 +591,102 @@
     <col min="10" max="10" width="33" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="165" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="165" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>33</v>
+      <c r="M2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="3">
+        <v>7854858555</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -660,8 +697,9 @@
     <hyperlink ref="J2" r:id="rId4" xr:uid="{305CCCEF-DD03-4C1C-B8FE-C8C910A7023A}"/>
     <hyperlink ref="K2" r:id="rId5" xr:uid="{20091B2C-B9BE-4658-A4F9-D8BC875D3128}"/>
     <hyperlink ref="L2" r:id="rId6" xr:uid="{67C4C0CE-3B0D-49FB-AB24-1B4326182702}"/>
+    <hyperlink ref="M2" r:id="rId7" xr:uid="{8C4E3D90-295F-492A-B753-9A83991A9586}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>